<commit_message>
added functionality to create item
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -3,24 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\javafx-restaurant-app\Group14-A2\src\main\java\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72A6DEB-7302-4913-924B-4A14783B969E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B2A894-BA7C-42F5-9B15-184CBE719CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="User Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Item Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Item Name</t>
   </si>
@@ -38,12 +38,16 @@
   </si>
   <si>
     <t>Item ID</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,13 +393,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5859375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.00390625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.47265625" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -441,6 +450,39 @@
         <v>30</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
created the create edit page
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\javafx-restaurant-app\Group14-A2\src\main\java\Items\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B2A894-BA7C-42F5-9B15-184CBE719CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7990C15D-DA4D-4336-A849-9D60578766AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="156" yWindow="1440" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Item Name</t>
   </si>
@@ -41,13 +41,18 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Special Item</t>
+  </si>
+  <si>
+    <t>Is Active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,9 +102,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -137,7 +142,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -243,7 +248,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,7 +390,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -393,20 +398,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5859375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.00390625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="5.47265625" collapsed="true"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -416,8 +421,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -427,8 +438,14 @@
       <c r="C2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -438,8 +455,14 @@
       <c r="C3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -449,38 +472,62 @@
       <c r="C4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4.0</v>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6.0</v>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="n">
-        <v>1.0</v>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made excel sheet editor better with 2 functuons using it
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7990C15D-DA4D-4336-A849-9D60578766AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAADA735-B053-403B-932C-46B1F97F26E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="156" yWindow="1440" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,6 +53,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,9 +407,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -469,11 +470,11 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>30</v>
+      <c r="C4" t="n">
+        <v>30.0</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -527,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added function to edit the orderstatus and the orders
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Item Name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Is Active</t>
+  </si>
+  <si>
+    <t>ice cream</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
@@ -407,9 +410,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="5.44140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5859375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.00390625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.47265625" collapsed="true"/>
+    <col min="4" max="4" width="11.93359375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="8.484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -494,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -511,7 +516,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -529,6 +534,23 @@
       </c>
       <c r="E7" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the final functionality for manager
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Item Name</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>ice cream</t>
+  </si>
+  <si>
+    <t>Pizza</t>
   </si>
 </sst>
 </file>
@@ -413,8 +416,8 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="7.5859375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.00390625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="5.47265625" collapsed="true"/>
-    <col min="4" max="4" width="11.93359375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="8.484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.93359375" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.484375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -490,10 +493,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.0</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
completed chef page and fixed bug in driver
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Item Name</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>Pizza</t>
+  </si>
+  <si>
+    <t>Naan</t>
+  </si>
+  <si>
+    <t>Biriyani</t>
+  </si>
+  <si>
+    <t>Steak</t>
+  </si>
+  <si>
+    <t>Noodles</t>
   </si>
 </sst>
 </file>
@@ -405,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
@@ -416,8 +428,8 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="7.5859375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.00390625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="5.47265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.93359375" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.484375" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.93359375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.484375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -510,13 +522,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5.0</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -527,10 +539,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.0</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -553,6 +565,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed the reservation system
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Item Name</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Noodles</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C4" t="n">
         <v>30.0</v>

</xml_diff>

<commit_message>
fixed bug with item edit
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Item Name</t>
   </si>
@@ -68,6 +68,24 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Green Tea</t>
+  </si>
+  <si>
+    <t>Mozzerella Stick</t>
+  </si>
+  <si>
+    <t>mozerella stick</t>
+  </si>
+  <si>
+    <t>m s</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>Roti</t>
   </si>
 </sst>
 </file>
@@ -420,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
@@ -429,7 +447,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="7.5859375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.00390625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="5.47265625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.93359375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="8.484375" collapsed="true"/>
@@ -457,10 +475,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10.0</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -602,6 +620,23 @@
         <v>0</v>
       </c>
       <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the new feature for chef item edit
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Item Name</t>
   </si>
@@ -494,11 +494,11 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>10</v>
+      <c r="C3" t="n">
+        <v>10.0</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Completed the chef page
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Items/ItemData.xlsx
+++ b/Group14-A2/src/main/java/Items/ItemData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Items\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\javafx-restaurant-app\Group14-A2\src\main\java\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAADA735-B053-403B-932C-46B1F97F26E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CD7699-C167-4413-A296-D1C0C5D08F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="156" yWindow="1440" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Item Name</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Tea</t>
-  </si>
-  <si>
     <t>Coffee</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>Item ID</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Special Item</t>
   </si>
   <si>
@@ -67,22 +61,7 @@
     <t>Noodles</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Green Tea</t>
-  </si>
-  <si>
-    <t>Mozzerella Stick</t>
-  </si>
-  <si>
-    <t>mozerella stick</t>
-  </si>
-  <si>
-    <t>m s</t>
-  </si>
-  <si>
-    <t>new</t>
   </si>
   <si>
     <t>Roti</t>
@@ -142,9 +121,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -182,7 +161,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -288,7 +267,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -430,7 +409,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,44 +420,44 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5859375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="5.47265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.93359375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.484375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.453125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="n">
-        <v>10.0</v>
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -487,15 +466,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="n">
-        <v>10.0</v>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -504,15 +483,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="n">
-        <v>30.0</v>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -521,32 +500,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.0</v>
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="n">
-        <v>5.0</v>
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -555,83 +534,83 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2.0</v>
+      <c r="C11">
+        <v>2</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>

</xml_diff>